<commit_message>
Block Global Vendor Script
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="43"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="44"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -56,8 +56,9 @@
     <sheet name="Credit Note With PO" sheetId="42" r:id="rId42"/>
     <sheet name="BlockGlobalClient" sheetId="47" r:id="rId43"/>
     <sheet name="BlockGlobalBrand" sheetId="48" r:id="rId44"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId45"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId46"/>
+    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId45"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId46"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId47"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="1047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="1051">
   <si>
     <t>Description</t>
   </si>
@@ -3210,6 +3211,18 @@
   </si>
   <si>
     <t>Radisson GRT</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>CompanyVendor Number</t>
+  </si>
+  <si>
+    <t>CompanyVendor Name</t>
+  </si>
+  <si>
+    <t>AARUN AASHIYANA</t>
   </si>
 </sst>
 </file>
@@ -3476,7 +3489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3676,6 +3689,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11118,14 +11134,14 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11175,6 +11191,69 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B3">
+        <v>107444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11407,7 +11486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>

</xml_diff>

<commit_message>
Datasheet Chanages for critical
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="44"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -3978,8 +3978,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4001,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="96" t="s">
-        <v>379</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11197,7 +11197,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -11494,7 +11494,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Block Company Product Script
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\Critical_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegpack\TestResource\Critical_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,9 +56,14 @@
     <sheet name="Credit Note With PO" sheetId="42" r:id="rId42"/>
     <sheet name="BlockGlobalClient" sheetId="47" r:id="rId43"/>
     <sheet name="BlockGlobalBrand" sheetId="48" r:id="rId44"/>
-    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId45"/>
-    <sheet name="Agency Users" sheetId="11" r:id="rId46"/>
-    <sheet name="SSC Users" sheetId="12" r:id="rId47"/>
+    <sheet name="BlockCompanyBrand" sheetId="50" r:id="rId45"/>
+    <sheet name="BlockCompanyClient" sheetId="51" r:id="rId46"/>
+    <sheet name="BlockGlobalProduct" sheetId="52" r:id="rId47"/>
+    <sheet name="BlockCompanyProduct" sheetId="53" r:id="rId48"/>
+    <sheet name="BlockGlobalVendor" sheetId="49" r:id="rId49"/>
+    <sheet name="BlockCompanyVendor" sheetId="54" r:id="rId50"/>
+    <sheet name="Agency Users" sheetId="11" r:id="rId51"/>
+    <sheet name="SSC Users" sheetId="12" r:id="rId52"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -70,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="1065">
   <si>
     <t>Description</t>
   </si>
@@ -3232,13 +3237,46 @@
   </si>
   <si>
     <t>103556</t>
+  </si>
+  <si>
+    <t>103132</t>
+  </si>
+  <si>
+    <t>103132002</t>
+  </si>
+  <si>
+    <t>Times Of India</t>
+  </si>
+  <si>
+    <t>Product Number</t>
+  </si>
+  <si>
+    <t>103132002001</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>NewCamlinProduct</t>
+  </si>
+  <si>
+    <t>103115001001</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>30 SECONDS OF FAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3283,6 +3321,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3498,7 +3543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3700,6 +3745,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4010,7 +4059,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="96" t="s">
-        <v>1010</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11228,48 +11277,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="43" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="B1" s="103">
         <v>1707</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B2">
-        <v>1707</v>
+        <v>1042</v>
+      </c>
+      <c r="B2" s="106" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B3">
-        <v>107444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B4" s="105" t="s">
-        <v>1050</v>
+        <v>1043</v>
+      </c>
+      <c r="B4" s="104" t="s">
+        <v>1055</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>1044</v>
       </c>
       <c r="B5" t="s">
-        <v>397</v>
+        <v>1056</v>
       </c>
     </row>
   </sheetData>
@@ -11281,229 +11330,43 @@
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="39">
-        <v>1707</v>
-      </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="97" t="s">
-        <v>964</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="97" t="s">
-        <v>965</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="B4" s="97" t="s">
-        <v>966</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="97" t="s">
-        <v>967</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="97" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" s="97" t="s">
-        <v>968</v>
-      </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" s="97" t="s">
-        <v>969</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="B9" s="97" t="s">
-        <v>970</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" s="97" t="s">
-        <v>971</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="98" t="s">
-        <v>972</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B2" s="106" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>397</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11514,138 +11377,184 @@
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="100" t="s">
-        <v>182</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="103">
+        <v>1707</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="97" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>1006</v>
+      <c r="A2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B2" s="1">
+        <v>103115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>1007</v>
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="97" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>1008</v>
+      <c r="A4" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B4" s="107" t="s">
+        <v>1061</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
-        <v>188</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="97" t="s">
-        <v>190</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="97" t="s">
-        <v>191</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="97" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="97" t="s">
-        <v>194</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="97" t="s">
-        <v>195</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="97" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="97" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="98" t="s">
-        <v>200</v>
-      </c>
-      <c r="B15" s="101" t="s">
-        <v>1019</v>
+      <c r="A5" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="103">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B2" s="107">
+        <v>103132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B4" s="107" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3">
+        <v>107433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -11876,6 +11785,442 @@
       <c r="C19" s="77"/>
       <c r="D19" s="77"/>
       <c r="E19" s="77"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B3">
+        <v>107444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="39">
+        <v>1707</v>
+      </c>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="97" t="s">
+        <v>964</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="97" t="s">
+        <v>965</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" s="97" t="s">
+        <v>966</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="97" t="s">
+        <v>967</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>379</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="97" t="s">
+        <v>968</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="97" t="s">
+        <v>969</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="97" t="s">
+        <v>970</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="97" t="s">
+        <v>971</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="98" t="s">
+        <v>972</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="100" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="97" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="97" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="97" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="97" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="97" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="97" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="97" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="97" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="97" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="98" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="101" t="s">
+        <v>1019</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in Global Client
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="42"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="39" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -3308,7 +3308,7 @@
     <t>No.2  Ward No.83</t>
   </si>
   <si>
-    <t>3543214645</t>
+    <t>3543214648</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Email code changes in Amend
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\Critical_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegpack\TestResource\Critical_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="42" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="1084">
   <si>
     <t>Description</t>
   </si>
@@ -3321,9 +3321,6 @@
   </si>
   <si>
     <t>Amended Global Client No</t>
-  </si>
-  <si>
-    <t>1707Auto1@gmail.com</t>
   </si>
   <si>
     <t>No.2  Ward No.83</t>
@@ -5614,7 +5611,7 @@
   </sheetPr>
   <dimension ref="A1:FK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B11:B22"/>
     </sheetView>
   </sheetViews>
@@ -5904,7 +5901,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>
@@ -11224,7 +11221,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11310,7 +11307,7 @@
         <v>1048</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -11465,7 +11462,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -11526,7 +11523,7 @@
         <v>1025</v>
       </c>
       <c r="B8" t="s">
-        <v>1081</v>
+        <v>1056</v>
       </c>
     </row>
   </sheetData>
@@ -11543,7 +11540,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11597,7 +11594,7 @@
         <v>1021</v>
       </c>
       <c r="B6" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -11620,7 +11617,7 @@
         <v>1025</v>
       </c>
       <c r="B10" t="s">
-        <v>1081</v>
+        <v>1056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Changes to CreateGlobalVendor
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -3336,12 +3336,6 @@
     <t>12 1st cross street</t>
   </si>
   <si>
-    <t>Automationvendor@gmail.com</t>
-  </si>
-  <si>
-    <t>AutomationVendor1</t>
-  </si>
-  <si>
     <t>Post</t>
   </si>
   <si>
@@ -3354,9 +3348,6 @@
     <t>Tax No</t>
   </si>
   <si>
-    <t>5698398649273</t>
-  </si>
-  <si>
     <t>CompRegNo</t>
   </si>
   <si>
@@ -3445,6 +3436,15 @@
   </si>
   <si>
     <t>WHMethod</t>
+  </si>
+  <si>
+    <t>Automationvendor1@yahoo.com</t>
+  </si>
+  <si>
+    <t>AutomationVendorTest1</t>
+  </si>
+  <si>
+    <t>586294318</t>
   </si>
 </sst>
 </file>
@@ -12422,8 +12422,8 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12461,7 +12461,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="101" t="s">
-        <v>1085</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -12485,12 +12485,12 @@
         <v>1004</v>
       </c>
       <c r="B7" t="s">
-        <v>1086</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="B8">
         <v>6000056</v>
@@ -12498,10 +12498,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B9" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -12514,26 +12514,26 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>1091</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="B12" s="60" t="s">
-        <v>1091</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="B13" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -12541,63 +12541,63 @@
         <v>1051</v>
       </c>
       <c r="B14" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="B15" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B16" t="s">
-        <v>1086</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B17" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="B18" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="B19" s="60" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B20" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="B21" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -12610,7 +12610,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B23" t="s">
         <v>1060</v>
@@ -12618,31 +12618,31 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="B24" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B25" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="B26" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="B27">
         <v>3000</v>
@@ -12650,7 +12650,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="B28">
         <v>300000</v>
@@ -12658,7 +12658,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="B29" t="s">
         <v>1003</v>
@@ -12666,15 +12666,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="B30" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="B31" t="s">
         <v>1069</v>
@@ -12682,23 +12682,23 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="B32" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="B33" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="B34" t="s">
         <v>313</v>

</xml_diff>

<commit_message>
DataSheet change - Server Config
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="51" activeTab="55"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -4243,8 +4243,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4266,7 +4266,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="94" t="s">
-        <v>958</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5761,7 +5761,7 @@
   </sheetPr>
   <dimension ref="A1:FK22"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -12819,7 +12819,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13073,7 +13073,7 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data Sheet changed For IndIA
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="43" activeTab="43"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="42" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1135">
   <si>
     <t>Description</t>
   </si>
@@ -3474,13 +3474,16 @@
     <t>No.2  Ward No.84</t>
   </si>
   <si>
-    <t>AutomUserEmail@gmail.com</t>
-  </si>
-  <si>
     <t>Radisson Bengaluru Citi</t>
   </si>
   <si>
     <t>AutoGlobalBrand 26February2020 15:15:49</t>
+  </si>
+  <si>
+    <t>No.2  Ward No.89</t>
+  </si>
+  <si>
+    <t>AutomUseroneEmail@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -11618,7 +11621,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11655,7 +11658,7 @@
         <v>1019</v>
       </c>
       <c r="B4" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11678,7 +11681,7 @@
         <v>1023</v>
       </c>
       <c r="B8" s="100" t="s">
-        <v>1131</v>
+        <v>1134</v>
       </c>
     </row>
   </sheetData>
@@ -11744,7 +11747,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -11838,7 +11841,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11884,7 +11887,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
   </sheetData>
@@ -13077,7 +13080,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed client number in ds
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="42" activeTab="43"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="42" activeTab="44"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -3474,9 +3474,6 @@
     <t>No.2  Ward No.84</t>
   </si>
   <si>
-    <t>Radisson Bengaluru Citi</t>
-  </si>
-  <si>
     <t>AutoGlobalBrand 26February2020 15:15:49</t>
   </si>
   <si>
@@ -3484,6 +3481,9 @@
   </si>
   <si>
     <t>AutoUseroneEmail@gmail.com</t>
+  </si>
+  <si>
+    <t>1707_AutoClient 27February2020 09:17:32</t>
   </si>
 </sst>
 </file>
@@ -11620,8 +11620,8 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11658,7 +11658,7 @@
         <v>1019</v>
       </c>
       <c r="B4" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11681,7 +11681,7 @@
         <v>1023</v>
       </c>
       <c r="B8" s="100" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
   </sheetData>
@@ -11700,8 +11700,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11747,7 +11747,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1131</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated critical regrssion datasheet
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="49" activeTab="52"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1135">
   <si>
     <t>Description</t>
   </si>
@@ -3469,9 +3469,6 @@
   </si>
   <si>
     <t>AutoGlobalBrand 26February2020 15:15:49</t>
-  </si>
-  <si>
-    <t>No.2  Ward No.86</t>
   </si>
   <si>
     <t>AutoUseroneEmail@gmail.com</t>
@@ -11623,13 +11620,14 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11661,7 +11659,7 @@
         <v>1019</v>
       </c>
       <c r="B4" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11684,7 +11682,7 @@
         <v>1023</v>
       </c>
       <c r="B8" s="100" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
   </sheetData>
@@ -11750,7 +11748,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -11758,7 +11756,7 @@
         <v>1019</v>
       </c>
       <c r="B6" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -11781,7 +11779,7 @@
         <v>1023</v>
       </c>
       <c r="B10" s="100" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
   </sheetData>
@@ -11807,6 +11805,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -11853,7 +11852,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -12469,7 +12468,7 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -12564,7 +12563,7 @@
         <v>1082</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -12572,7 +12571,7 @@
         <v>1083</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made change to Amend Global Vendor
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="43" activeTab="45"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1137">
   <si>
     <t>Description</t>
   </si>
@@ -3420,12 +3420,6 @@
     <t>WHMethod</t>
   </si>
   <si>
-    <t>Automationvendor1@yahoo.com</t>
-  </si>
-  <si>
-    <t>AutomationVendorTest1</t>
-  </si>
-  <si>
     <t>107758</t>
   </si>
   <si>
@@ -3477,16 +3471,25 @@
     <t>AutomoneEmail@gmail.com</t>
   </si>
   <si>
-    <t>586296666</t>
-  </si>
-  <si>
-    <t>No.2  Ward No.8567</t>
-  </si>
-  <si>
-    <t>AutoUseroneeEmail@gmail.com</t>
-  </si>
-  <si>
     <t>No.2  Ward No.83343</t>
+  </si>
+  <si>
+    <t>8796504345</t>
+  </si>
+  <si>
+    <t>GlobalVendor</t>
+  </si>
+  <si>
+    <t>HDFC</t>
+  </si>
+  <si>
+    <t>Automationglobalvendor@yahoo.com</t>
+  </si>
+  <si>
+    <t>No.2  Ward No.4545</t>
+  </si>
+  <si>
+    <t>AutoUseroneEmail@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -4249,8 +4252,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,7 +4275,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="94" t="s">
-        <v>362</v>
+        <v>958</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11624,7 +11627,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11646,7 +11649,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11662,7 +11665,7 @@
         <v>1019</v>
       </c>
       <c r="B4" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11685,7 +11688,7 @@
         <v>1023</v>
       </c>
       <c r="B8" s="100" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
     </row>
   </sheetData>
@@ -11727,7 +11730,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11743,7 +11746,7 @@
         <v>985</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11751,7 +11754,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -11759,7 +11762,7 @@
         <v>1019</v>
       </c>
       <c r="B6" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -11782,7 +11785,7 @@
         <v>1023</v>
       </c>
       <c r="B10" s="100" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
   </sheetData>
@@ -11801,8 +11804,8 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11824,7 +11827,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11871,7 +11874,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11887,7 +11890,7 @@
         <v>985</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11895,7 +11898,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
   </sheetData>
@@ -12471,8 +12474,8 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12510,7 +12513,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="100" t="s">
-        <v>1113</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -12534,7 +12537,7 @@
         <v>1002</v>
       </c>
       <c r="B7" t="s">
-        <v>1114</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -12566,7 +12569,7 @@
         <v>1082</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -12574,7 +12577,7 @@
         <v>1083</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -12606,7 +12609,7 @@
         <v>1089</v>
       </c>
       <c r="B16" t="s">
-        <v>1114</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -12833,7 +12836,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12872,7 +12875,7 @@
         <v>942</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
@@ -12893,7 +12896,7 @@
         <v>943</v>
       </c>
       <c r="C3" s="95" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -12914,7 +12917,7 @@
         <v>944</v>
       </c>
       <c r="C4" s="95" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
@@ -12935,7 +12938,7 @@
         <v>945</v>
       </c>
       <c r="C5" s="95" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
@@ -12956,7 +12959,7 @@
         <v>362</v>
       </c>
       <c r="C6" s="95" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
@@ -12977,7 +12980,7 @@
         <v>946</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
@@ -12998,7 +13001,7 @@
         <v>947</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
@@ -13019,7 +13022,7 @@
         <v>948</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -13040,7 +13043,7 @@
         <v>949</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
@@ -13061,7 +13064,7 @@
         <v>950</v>
       </c>
       <c r="C11" s="96" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>

</xml_diff>

<commit_message>
Create Amend Block Global Client Changes
</commit_message>
<xml_diff>
--- a/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
+++ b/WppRegpack/TestResource/Critical_Regression/DS_IND_CRITICAL_REGRESSION.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\662494\Pictures\Test_Environment_25-2-2020\GlobalTestSuiteAutomation\WppRegpack\TestResource\Critical_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\WppRegPack\TestResource\Critical_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="42" activeTab="43"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6720" firstSheet="41" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="Server Details" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="1137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="1144">
   <si>
     <t>Description</t>
   </si>
@@ -3312,9 +3312,6 @@
     <t>Amended Global Brand No</t>
   </si>
   <si>
-    <t>3543224601</t>
-  </si>
-  <si>
     <t>12 1st cross street</t>
   </si>
   <si>
@@ -3490,6 +3487,30 @@
   </si>
   <si>
     <t>No.2  Ward No.8456</t>
+  </si>
+  <si>
+    <t>1707105271</t>
+  </si>
+  <si>
+    <t>3543224602</t>
+  </si>
+  <si>
+    <t>107762</t>
+  </si>
+  <si>
+    <t>1707_AutoClient 04March2020 16:24:02</t>
+  </si>
+  <si>
+    <t>107762001</t>
+  </si>
+  <si>
+    <t>AutoGlobalBrand 04March2020 16:24:02</t>
+  </si>
+  <si>
+    <t>107762001001</t>
+  </si>
+  <si>
+    <t>AutoGlobalProduct 04March2020 16:24:02</t>
   </si>
 </sst>
 </file>
@@ -4253,7 +4274,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5771,7 +5792,7 @@
   <dimension ref="A1:FK22"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,6 +5981,9 @@
       <c r="A2" s="30" t="s">
         <v>197</v>
       </c>
+      <c r="B2" s="30" t="s">
+        <v>1136</v>
+      </c>
       <c r="C2" s="59"/>
       <c r="E2" s="59"/>
       <c r="F2" s="60"/>
@@ -6012,11 +6036,17 @@
       <c r="A11" s="30" t="s">
         <v>991</v>
       </c>
+      <c r="B11" s="30" t="s">
+        <v>1140</v>
+      </c>
     </row>
     <row r="12" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>992</v>
       </c>
+      <c r="B12" s="30" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="13" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
@@ -6027,43 +6057,67 @@
       <c r="A14" s="30" t="s">
         <v>1069</v>
       </c>
+      <c r="B14" s="30" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="15" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>1070</v>
       </c>
+      <c r="B15" s="30" t="s">
+        <v>1139</v>
+      </c>
     </row>
     <row r="16" spans="1:167" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>1071</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="30" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>1072</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>1073</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="30" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>1074</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="30" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>1075</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>1076</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="30" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>218</v>
       </c>
@@ -11384,8 +11438,8 @@
   </sheetPr>
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11471,7 +11525,7 @@
         <v>1043</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>1077</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -11626,7 +11680,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -11649,7 +11703,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11665,7 +11719,7 @@
         <v>1019</v>
       </c>
       <c r="B4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11688,7 +11742,7 @@
         <v>1023</v>
       </c>
       <c r="B8" s="100" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
   </sheetData>
@@ -11730,7 +11784,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11746,7 +11800,7 @@
         <v>985</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11754,7 +11808,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -11762,7 +11816,7 @@
         <v>1019</v>
       </c>
       <c r="B6" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -11785,7 +11839,7 @@
         <v>1023</v>
       </c>
       <c r="B10" s="100" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
   </sheetData>
@@ -11827,7 +11881,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11874,7 +11928,7 @@
         <v>984</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -11890,7 +11944,7 @@
         <v>985</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11898,7 +11952,7 @@
         <v>986</v>
       </c>
       <c r="B5" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
   </sheetData>
@@ -12024,8 +12078,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12505,7 +12559,7 @@
         <v>1035</v>
       </c>
       <c r="B3" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -12513,7 +12567,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="100" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -12537,12 +12591,12 @@
         <v>1002</v>
       </c>
       <c r="B7" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B8">
         <v>6000056</v>
@@ -12550,10 +12604,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B9" t="s">
         <v>1080</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -12566,26 +12620,26 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B13" t="s">
         <v>1084</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -12593,63 +12647,63 @@
         <v>1046</v>
       </c>
       <c r="B14" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B15" t="s">
         <v>1087</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B16" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B17" t="s">
         <v>1090</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B18" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B19" s="59" t="s">
         <v>1093</v>
-      </c>
-      <c r="B19" s="59" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B21" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -12662,7 +12716,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B23" t="s">
         <v>1055</v>
@@ -12670,31 +12724,31 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B24" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B25" t="s">
         <v>1099</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1100</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B26" t="s">
         <v>1101</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B27">
         <v>3000</v>
@@ -12702,7 +12756,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B28">
         <v>300000</v>
@@ -12710,7 +12764,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B29" t="s">
         <v>1001</v>
@@ -12718,15 +12772,15 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B30" t="s">
         <v>1106</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B31" t="s">
         <v>1064</v>
@@ -12734,23 +12788,23 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B32" t="s">
         <v>1109</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B33" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B34" t="s">
         <v>313</v>
@@ -12875,7 +12929,7 @@
         <v>942</v>
       </c>
       <c r="C2" s="95" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="38"/>
@@ -12896,7 +12950,7 @@
         <v>943</v>
       </c>
       <c r="C3" s="95" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -12917,7 +12971,7 @@
         <v>944</v>
       </c>
       <c r="C4" s="95" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
@@ -12938,7 +12992,7 @@
         <v>945</v>
       </c>
       <c r="C5" s="95" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
@@ -12959,7 +13013,7 @@
         <v>362</v>
       </c>
       <c r="C6" s="95" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
@@ -12980,7 +13034,7 @@
         <v>946</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
@@ -13001,7 +13055,7 @@
         <v>947</v>
       </c>
       <c r="C8" s="95" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
@@ -13022,7 +13076,7 @@
         <v>948</v>
       </c>
       <c r="C9" s="95" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -13043,7 +13097,7 @@
         <v>949</v>
       </c>
       <c r="C10" s="95" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
@@ -13064,7 +13118,7 @@
         <v>950</v>
       </c>
       <c r="C11" s="96" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>

</xml_diff>